<commit_message>
Modifica test 32 e 40
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix-xis/v3_19_05/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix-xis/v3_19_05/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACCREDITAMENTO_FSE\GATEWAY\A1#111ELCO0000000\EL_CO_\Fenix-xis\v3_19_05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAFBCBF-9B7F-41DF-8391-B3975632B8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA858CD4-5EC3-4352-A350-E3EA607A42D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-192" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5385" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2231" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="925">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4425,17 +4425,6 @@
     <t>Rivalidazione in Backoffice</t>
   </si>
   <si>
-    <t>title=AuthorizationContentDeny, status=403, detail=Unauthorized request content, govway_id=46dadc5a-f3e2-11ed-8882-005056ae54fa
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
-    <t>2023-05-16T13:23:10.656Z</t>
-  </si>
-  <si>
-    <t>title=AuthorizationContentDeny, status=403, detail=Unauthorized request content, govway_id=61d8a9ab-f3e6-11ed-80ae-005056ae7395 
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
     <t>Il sistema attende un numero di millisecondi configurabile (default 5000) Dopo tale tempo viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
   </si>
   <si>
@@ -4700,6 +4689,26 @@
   </si>
   <si>
     <t>3da1a208c48894f9</t>
+  </si>
+  <si>
+    <t>UNKNOWN_WORKFLOW_ID</t>
+  </si>
+  <si>
+    <t>9dcdbaaa9b0a140e</t>
+  </si>
+  <si>
+    <t>Il campo purpose_of_use non è valorizzato
+Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
+  </si>
+  <si>
+    <t>ee2620354d738c3f</t>
+  </si>
+  <si>
+    <t>2023-05-18T10:59:07.434Z</t>
+  </si>
+  <si>
+    <t>Il campo action_id non è corretto
+Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
   </si>
 </sst>
 </file>
@@ -5115,6 +5124,15 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5136,15 +5154,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7604,10 +7613,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="E350" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G351" sqref="G351"/>
+      <selection pane="bottomRight" activeCell="M231" sqref="M231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7646,12 +7655,12 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="36"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="39"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -7669,14 +7678,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="44" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="47" t="s">
         <v>829</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="39"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -7694,12 +7703,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="44" t="s">
+      <c r="A4" s="43"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="47" t="s">
         <v>830</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -7718,12 +7727,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="42"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="44" t="s">
+      <c r="A5" s="45"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47" t="s">
         <v>831</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="39"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -7741,8 +7750,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -7797,7 +7806,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="14.25" customHeight="1">
+    <row r="9" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
       <c r="A9" s="17" t="s">
         <v>24</v>
       </c>
@@ -14829,7 +14838,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="150">
+    <row r="215" spans="1:20" ht="150.75" thickBot="1">
       <c r="A215" s="20">
         <v>32</v>
       </c>
@@ -14846,13 +14855,17 @@
         <v>464</v>
       </c>
       <c r="F215" s="23">
-        <v>45062</v>
+        <v>45064</v>
       </c>
       <c r="G215" s="24" t="s">
         <v>832</v>
       </c>
-      <c r="H215" s="24"/>
-      <c r="I215" s="24"/>
+      <c r="H215" s="24" t="s">
+        <v>920</v>
+      </c>
+      <c r="I215" s="24" t="s">
+        <v>919</v>
+      </c>
       <c r="J215" s="25" t="s">
         <v>488</v>
       </c>
@@ -14864,7 +14877,7 @@
         <v>488</v>
       </c>
       <c r="N215" s="25" t="s">
-        <v>835</v>
+        <v>921</v>
       </c>
       <c r="O215" s="25" t="s">
         <v>833</v>
@@ -15117,7 +15130,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="165">
+    <row r="223" spans="1:20" ht="165.75" thickBot="1">
       <c r="A223" s="20">
         <v>40</v>
       </c>
@@ -15134,13 +15147,17 @@
         <v>472</v>
       </c>
       <c r="F223" s="23">
-        <v>45062</v>
+        <v>45064</v>
       </c>
       <c r="G223" s="24" t="s">
-        <v>836</v>
-      </c>
-      <c r="H223" s="24"/>
-      <c r="I223" s="24"/>
+        <v>923</v>
+      </c>
+      <c r="H223" s="24" t="s">
+        <v>922</v>
+      </c>
+      <c r="I223" s="24" t="s">
+        <v>919</v>
+      </c>
       <c r="J223" s="25" t="s">
         <v>488</v>
       </c>
@@ -15151,8 +15168,8 @@
       <c r="M223" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="N223" s="45" t="s">
-        <v>837</v>
+      <c r="N223" s="33" t="s">
+        <v>924</v>
       </c>
       <c r="O223" s="25" t="s">
         <v>833</v>
@@ -15167,7 +15184,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="165" hidden="1">
+    <row r="224" spans="1:20" ht="165" hidden="1" customHeight="1">
       <c r="A224" s="20">
         <v>41</v>
       </c>
@@ -15413,7 +15430,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="120">
+    <row r="231" spans="1:20" ht="120.75" thickBot="1">
       <c r="A231" s="20">
         <v>48</v>
       </c>
@@ -15433,7 +15450,7 @@
         <v>45062</v>
       </c>
       <c r="G231" s="24" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="H231" s="24"/>
       <c r="I231" s="24"/>
@@ -15447,8 +15464,8 @@
       <c r="M231" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="N231" s="45" t="s">
-        <v>838</v>
+      <c r="N231" s="33" t="s">
+        <v>835</v>
       </c>
       <c r="O231" s="25" t="s">
         <v>833</v>
@@ -18803,7 +18820,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="330" spans="1:20" ht="165">
+    <row r="330" spans="1:20" ht="165.75" thickBot="1">
       <c r="A330" s="20">
         <v>147</v>
       </c>
@@ -18823,13 +18840,13 @@
         <v>45062</v>
       </c>
       <c r="G330" s="24" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="H330" s="24" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="I330" s="24" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="J330" s="25" t="s">
         <v>488</v>
@@ -18847,7 +18864,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="331" spans="1:20" ht="165">
+    <row r="331" spans="1:20" ht="165.75" thickBot="1">
       <c r="A331" s="20">
         <v>148</v>
       </c>
@@ -18870,8 +18887,8 @@
       <c r="J331" s="25" t="s">
         <v>828</v>
       </c>
-      <c r="K331" s="45" t="s">
-        <v>844</v>
+      <c r="K331" s="33" t="s">
+        <v>841</v>
       </c>
       <c r="L331" s="25"/>
       <c r="M331" s="25"/>
@@ -18909,7 +18926,7 @@
         <v>828</v>
       </c>
       <c r="K332" s="25" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="L332" s="25"/>
       <c r="M332" s="25"/>
@@ -18947,7 +18964,7 @@
         <v>828</v>
       </c>
       <c r="K333" s="25" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="L333" s="25"/>
       <c r="M333" s="25"/>
@@ -18971,7 +18988,7 @@
       <c r="C334" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D334" s="46" t="s">
+      <c r="D334" s="34" t="s">
         <v>694</v>
       </c>
       <c r="E334" s="22" t="s">
@@ -18980,14 +18997,14 @@
       <c r="F334" s="23">
         <v>45062</v>
       </c>
-      <c r="G334" s="47" t="s">
-        <v>845</v>
-      </c>
-      <c r="H334" s="47" t="s">
-        <v>846</v>
-      </c>
-      <c r="I334" s="47" t="s">
-        <v>847</v>
+      <c r="G334" s="35" t="s">
+        <v>842</v>
+      </c>
+      <c r="H334" s="35" t="s">
+        <v>843</v>
+      </c>
+      <c r="I334" s="35" t="s">
+        <v>844</v>
       </c>
       <c r="J334" s="25" t="s">
         <v>488</v>
@@ -18999,14 +19016,14 @@
       <c r="M334" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="N334" s="45" t="s">
-        <v>851</v>
+      <c r="N334" s="33" t="s">
+        <v>848</v>
       </c>
       <c r="O334" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P334" s="45" t="s">
-        <v>857</v>
+      <c r="P334" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q334" s="25"/>
       <c r="R334" s="26"/>
@@ -19035,32 +19052,32 @@
         <v>45062</v>
       </c>
       <c r="G335" s="24" t="s">
-        <v>848</v>
-      </c>
-      <c r="H335" s="47" t="s">
+        <v>845</v>
+      </c>
+      <c r="H335" s="35" t="s">
+        <v>846</v>
+      </c>
+      <c r="I335" s="35" t="s">
+        <v>847</v>
+      </c>
+      <c r="J335" s="33" t="s">
+        <v>488</v>
+      </c>
+      <c r="K335" s="25"/>
+      <c r="L335" s="33" t="s">
+        <v>828</v>
+      </c>
+      <c r="M335" s="33" t="s">
+        <v>488</v>
+      </c>
+      <c r="N335" s="25" t="s">
         <v>849</v>
-      </c>
-      <c r="I335" s="47" t="s">
-        <v>850</v>
-      </c>
-      <c r="J335" s="45" t="s">
-        <v>488</v>
-      </c>
-      <c r="K335" s="25"/>
-      <c r="L335" s="45" t="s">
-        <v>828</v>
-      </c>
-      <c r="M335" s="45" t="s">
-        <v>488</v>
-      </c>
-      <c r="N335" s="25" t="s">
-        <v>852</v>
       </c>
       <c r="O335" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P335" s="45" t="s">
-        <v>857</v>
+      <c r="P335" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q335" s="25"/>
       <c r="R335" s="26"/>
@@ -19088,33 +19105,33 @@
       <c r="F336" s="23">
         <v>45062</v>
       </c>
-      <c r="G336" s="47" t="s">
-        <v>854</v>
-      </c>
-      <c r="H336" s="47" t="s">
-        <v>855</v>
-      </c>
-      <c r="I336" s="47" t="s">
-        <v>856</v>
-      </c>
-      <c r="J336" s="45" t="s">
+      <c r="G336" s="35" t="s">
+        <v>851</v>
+      </c>
+      <c r="H336" s="35" t="s">
+        <v>852</v>
+      </c>
+      <c r="I336" s="35" t="s">
+        <v>853</v>
+      </c>
+      <c r="J336" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K336" s="25"/>
-      <c r="L336" s="45" t="s">
+      <c r="L336" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M336" s="45" t="s">
+      <c r="M336" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N336" s="45" t="s">
-        <v>853</v>
+      <c r="N336" s="33" t="s">
+        <v>850</v>
       </c>
       <c r="O336" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P336" s="45" t="s">
-        <v>857</v>
+      <c r="P336" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q336" s="25"/>
       <c r="R336" s="26"/>
@@ -19142,33 +19159,33 @@
       <c r="F337" s="23">
         <v>45062</v>
       </c>
-      <c r="G337" s="47" t="s">
-        <v>860</v>
-      </c>
-      <c r="H337" s="47" t="s">
-        <v>859</v>
-      </c>
-      <c r="I337" s="47" t="s">
-        <v>861</v>
-      </c>
-      <c r="J337" s="45" t="s">
+      <c r="G337" s="35" t="s">
+        <v>857</v>
+      </c>
+      <c r="H337" s="35" t="s">
+        <v>856</v>
+      </c>
+      <c r="I337" s="35" t="s">
+        <v>858</v>
+      </c>
+      <c r="J337" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K337" s="25"/>
-      <c r="L337" s="45" t="s">
+      <c r="L337" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M337" s="45" t="s">
+      <c r="M337" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N337" s="45" t="s">
-        <v>858</v>
+      <c r="N337" s="33" t="s">
+        <v>855</v>
       </c>
       <c r="O337" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P337" s="45" t="s">
-        <v>857</v>
+      <c r="P337" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q337" s="25"/>
       <c r="R337" s="26"/>
@@ -19196,33 +19213,33 @@
       <c r="F338" s="23">
         <v>45062</v>
       </c>
-      <c r="G338" s="47" t="s">
-        <v>865</v>
-      </c>
-      <c r="H338" s="47" t="s">
-        <v>864</v>
-      </c>
-      <c r="I338" s="47" t="s">
-        <v>863</v>
-      </c>
-      <c r="J338" s="45" t="s">
+      <c r="G338" s="35" t="s">
+        <v>862</v>
+      </c>
+      <c r="H338" s="35" t="s">
+        <v>861</v>
+      </c>
+      <c r="I338" s="35" t="s">
+        <v>860</v>
+      </c>
+      <c r="J338" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K338" s="25"/>
-      <c r="L338" s="45" t="s">
+      <c r="L338" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M338" s="45" t="s">
+      <c r="M338" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N338" s="45" t="s">
-        <v>862</v>
+      <c r="N338" s="33" t="s">
+        <v>859</v>
       </c>
       <c r="O338" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P338" s="45" t="s">
-        <v>857</v>
+      <c r="P338" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q338" s="25"/>
       <c r="R338" s="26"/>
@@ -19250,33 +19267,33 @@
       <c r="F339" s="23">
         <v>45062</v>
       </c>
-      <c r="G339" s="47" t="s">
-        <v>867</v>
+      <c r="G339" s="35" t="s">
+        <v>864</v>
       </c>
       <c r="H339" s="24" t="s">
-        <v>869</v>
-      </c>
-      <c r="I339" s="47" t="s">
-        <v>868</v>
-      </c>
-      <c r="J339" s="45" t="s">
+        <v>866</v>
+      </c>
+      <c r="I339" s="35" t="s">
+        <v>865</v>
+      </c>
+      <c r="J339" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K339" s="25"/>
-      <c r="L339" s="45" t="s">
+      <c r="L339" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M339" s="45" t="s">
+      <c r="M339" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N339" s="45" t="s">
-        <v>866</v>
+      <c r="N339" s="33" t="s">
+        <v>863</v>
       </c>
       <c r="O339" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P339" s="45" t="s">
-        <v>857</v>
+      <c r="P339" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q339" s="25"/>
       <c r="R339" s="26"/>
@@ -19305,32 +19322,32 @@
         <v>45062</v>
       </c>
       <c r="G340" s="24" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="H340" s="24" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="I340" s="24" t="s">
-        <v>871</v>
-      </c>
-      <c r="J340" s="45" t="s">
+        <v>868</v>
+      </c>
+      <c r="J340" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K340" s="25"/>
-      <c r="L340" s="45" t="s">
+      <c r="L340" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M340" s="45" t="s">
+      <c r="M340" s="33" t="s">
         <v>488</v>
       </c>
       <c r="N340" s="25" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="O340" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P340" s="45" t="s">
-        <v>857</v>
+      <c r="P340" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q340" s="25"/>
       <c r="R340" s="26"/>
@@ -19358,33 +19375,33 @@
       <c r="F341" s="23">
         <v>45062</v>
       </c>
-      <c r="G341" s="47" t="s">
-        <v>877</v>
-      </c>
-      <c r="H341" s="47" t="s">
-        <v>876</v>
-      </c>
-      <c r="I341" s="47" t="s">
-        <v>875</v>
-      </c>
-      <c r="J341" s="45" t="s">
+      <c r="G341" s="35" t="s">
+        <v>874</v>
+      </c>
+      <c r="H341" s="35" t="s">
+        <v>873</v>
+      </c>
+      <c r="I341" s="35" t="s">
+        <v>872</v>
+      </c>
+      <c r="J341" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K341" s="25"/>
-      <c r="L341" s="45" t="s">
+      <c r="L341" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M341" s="45" t="s">
+      <c r="M341" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N341" s="45" t="s">
-        <v>874</v>
+      <c r="N341" s="33" t="s">
+        <v>871</v>
       </c>
       <c r="O341" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P341" s="45" t="s">
-        <v>857</v>
+      <c r="P341" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q341" s="25"/>
       <c r="R341" s="26"/>
@@ -19412,33 +19429,33 @@
       <c r="F342" s="23">
         <v>45062</v>
       </c>
-      <c r="G342" s="47" t="s">
-        <v>881</v>
-      </c>
-      <c r="H342" s="47" t="s">
-        <v>880</v>
-      </c>
-      <c r="I342" s="47" t="s">
-        <v>879</v>
-      </c>
-      <c r="J342" s="45" t="s">
+      <c r="G342" s="35" t="s">
+        <v>878</v>
+      </c>
+      <c r="H342" s="35" t="s">
+        <v>877</v>
+      </c>
+      <c r="I342" s="35" t="s">
+        <v>876</v>
+      </c>
+      <c r="J342" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K342" s="25"/>
-      <c r="L342" s="45" t="s">
+      <c r="L342" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M342" s="45" t="s">
+      <c r="M342" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N342" s="45" t="s">
-        <v>878</v>
+      <c r="N342" s="33" t="s">
+        <v>875</v>
       </c>
       <c r="O342" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P342" s="45" t="s">
-        <v>857</v>
+      <c r="P342" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q342" s="25"/>
       <c r="R342" s="26"/>
@@ -19466,33 +19483,33 @@
       <c r="F343" s="23">
         <v>45062</v>
       </c>
-      <c r="G343" s="47" t="s">
-        <v>885</v>
-      </c>
-      <c r="H343" s="47" t="s">
-        <v>884</v>
-      </c>
-      <c r="I343" s="47" t="s">
-        <v>883</v>
-      </c>
-      <c r="J343" s="45" t="s">
+      <c r="G343" s="35" t="s">
+        <v>882</v>
+      </c>
+      <c r="H343" s="35" t="s">
+        <v>881</v>
+      </c>
+      <c r="I343" s="35" t="s">
+        <v>880</v>
+      </c>
+      <c r="J343" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K343" s="25"/>
-      <c r="L343" s="45" t="s">
+      <c r="L343" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M343" s="45" t="s">
+      <c r="M343" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N343" s="45" t="s">
-        <v>882</v>
+      <c r="N343" s="33" t="s">
+        <v>879</v>
       </c>
       <c r="O343" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P343" s="45" t="s">
-        <v>857</v>
+      <c r="P343" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q343" s="25"/>
       <c r="R343" s="26"/>
@@ -19520,33 +19537,33 @@
       <c r="F344" s="23">
         <v>45062</v>
       </c>
-      <c r="G344" s="47" t="s">
-        <v>889</v>
-      </c>
-      <c r="H344" s="47" t="s">
-        <v>888</v>
-      </c>
-      <c r="I344" s="47" t="s">
-        <v>887</v>
-      </c>
-      <c r="J344" s="45" t="s">
+      <c r="G344" s="35" t="s">
+        <v>886</v>
+      </c>
+      <c r="H344" s="35" t="s">
+        <v>885</v>
+      </c>
+      <c r="I344" s="35" t="s">
+        <v>884</v>
+      </c>
+      <c r="J344" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K344" s="25"/>
-      <c r="L344" s="45" t="s">
+      <c r="L344" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M344" s="45" t="s">
+      <c r="M344" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N344" s="45" t="s">
-        <v>886</v>
+      <c r="N344" s="33" t="s">
+        <v>883</v>
       </c>
       <c r="O344" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P344" s="45" t="s">
-        <v>857</v>
+      <c r="P344" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q344" s="25"/>
       <c r="R344" s="26"/>
@@ -19574,33 +19591,33 @@
       <c r="F345" s="23">
         <v>45062</v>
       </c>
-      <c r="G345" s="47" t="s">
-        <v>893</v>
-      </c>
-      <c r="H345" s="47" t="s">
-        <v>892</v>
-      </c>
-      <c r="I345" s="47" t="s">
-        <v>891</v>
-      </c>
-      <c r="J345" s="45" t="s">
+      <c r="G345" s="35" t="s">
+        <v>890</v>
+      </c>
+      <c r="H345" s="35" t="s">
+        <v>889</v>
+      </c>
+      <c r="I345" s="35" t="s">
+        <v>888</v>
+      </c>
+      <c r="J345" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K345" s="25"/>
-      <c r="L345" s="45" t="s">
+      <c r="L345" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M345" s="45" t="s">
+      <c r="M345" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N345" s="45" t="s">
-        <v>890</v>
+      <c r="N345" s="33" t="s">
+        <v>887</v>
       </c>
       <c r="O345" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P345" s="45" t="s">
-        <v>857</v>
+      <c r="P345" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q345" s="25"/>
       <c r="R345" s="26"/>
@@ -19628,33 +19645,33 @@
       <c r="F346" s="23">
         <v>45062</v>
       </c>
-      <c r="G346" s="47" t="s">
-        <v>897</v>
-      </c>
-      <c r="H346" s="47" t="s">
-        <v>896</v>
-      </c>
-      <c r="I346" s="47" t="s">
-        <v>895</v>
-      </c>
-      <c r="J346" s="45" t="s">
+      <c r="G346" s="35" t="s">
+        <v>894</v>
+      </c>
+      <c r="H346" s="35" t="s">
+        <v>893</v>
+      </c>
+      <c r="I346" s="35" t="s">
+        <v>892</v>
+      </c>
+      <c r="J346" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K346" s="25"/>
-      <c r="L346" s="45" t="s">
+      <c r="L346" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M346" s="45" t="s">
+      <c r="M346" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N346" s="45" t="s">
-        <v>894</v>
+      <c r="N346" s="33" t="s">
+        <v>891</v>
       </c>
       <c r="O346" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P346" s="45" t="s">
-        <v>857</v>
+      <c r="P346" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q346" s="25"/>
       <c r="R346" s="26"/>
@@ -19682,33 +19699,33 @@
       <c r="F347" s="23">
         <v>45062</v>
       </c>
-      <c r="G347" s="47" t="s">
-        <v>901</v>
-      </c>
-      <c r="H347" s="47" t="s">
-        <v>900</v>
-      </c>
-      <c r="I347" s="47" t="s">
-        <v>899</v>
-      </c>
-      <c r="J347" s="45" t="s">
+      <c r="G347" s="35" t="s">
+        <v>898</v>
+      </c>
+      <c r="H347" s="35" t="s">
+        <v>897</v>
+      </c>
+      <c r="I347" s="35" t="s">
+        <v>896</v>
+      </c>
+      <c r="J347" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K347" s="25"/>
-      <c r="L347" s="45" t="s">
+      <c r="L347" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M347" s="45" t="s">
+      <c r="M347" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N347" s="45" t="s">
-        <v>898</v>
+      <c r="N347" s="33" t="s">
+        <v>895</v>
       </c>
       <c r="O347" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P347" s="45" t="s">
-        <v>857</v>
+      <c r="P347" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q347" s="25"/>
       <c r="R347" s="26"/>
@@ -19736,33 +19753,33 @@
       <c r="F348" s="23">
         <v>45062</v>
       </c>
-      <c r="G348" s="47" t="s">
-        <v>905</v>
-      </c>
-      <c r="H348" s="47" t="s">
-        <v>904</v>
-      </c>
-      <c r="I348" s="47" t="s">
-        <v>903</v>
-      </c>
-      <c r="J348" s="45" t="s">
+      <c r="G348" s="35" t="s">
+        <v>902</v>
+      </c>
+      <c r="H348" s="35" t="s">
+        <v>901</v>
+      </c>
+      <c r="I348" s="35" t="s">
+        <v>900</v>
+      </c>
+      <c r="J348" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K348" s="25"/>
-      <c r="L348" s="45" t="s">
+      <c r="L348" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M348" s="45" t="s">
+      <c r="M348" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N348" s="45" t="s">
-        <v>902</v>
+      <c r="N348" s="33" t="s">
+        <v>899</v>
       </c>
       <c r="O348" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P348" s="45" t="s">
-        <v>857</v>
+      <c r="P348" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q348" s="25"/>
       <c r="R348" s="26"/>
@@ -19790,33 +19807,33 @@
       <c r="F349" s="23">
         <v>45062</v>
       </c>
-      <c r="G349" s="47" t="s">
-        <v>909</v>
-      </c>
-      <c r="H349" s="47" t="s">
-        <v>908</v>
-      </c>
-      <c r="I349" s="47" t="s">
-        <v>907</v>
-      </c>
-      <c r="J349" s="45" t="s">
+      <c r="G349" s="35" t="s">
+        <v>906</v>
+      </c>
+      <c r="H349" s="35" t="s">
+        <v>905</v>
+      </c>
+      <c r="I349" s="35" t="s">
+        <v>904</v>
+      </c>
+      <c r="J349" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K349" s="25"/>
-      <c r="L349" s="45" t="s">
+      <c r="L349" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M349" s="45" t="s">
+      <c r="M349" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N349" s="45" t="s">
-        <v>906</v>
+      <c r="N349" s="33" t="s">
+        <v>903</v>
       </c>
       <c r="O349" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P349" s="45" t="s">
-        <v>857</v>
+      <c r="P349" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q349" s="25"/>
       <c r="R349" s="26"/>
@@ -19845,32 +19862,32 @@
         <v>45062</v>
       </c>
       <c r="G350" s="24" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="H350" s="24" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="I350" s="24" t="s">
-        <v>911</v>
-      </c>
-      <c r="J350" s="45" t="s">
+        <v>908</v>
+      </c>
+      <c r="J350" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K350" s="25"/>
-      <c r="L350" s="45" t="s">
+      <c r="L350" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M350" s="45" t="s">
+      <c r="M350" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N350" s="45" t="s">
-        <v>910</v>
+      <c r="N350" s="33" t="s">
+        <v>907</v>
       </c>
       <c r="O350" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P350" s="45" t="s">
-        <v>857</v>
+      <c r="P350" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q350" s="25"/>
       <c r="R350" s="26"/>
@@ -19898,33 +19915,33 @@
       <c r="F351" s="23">
         <v>45062</v>
       </c>
-      <c r="G351" s="47" t="s">
-        <v>917</v>
-      </c>
-      <c r="H351" s="47" t="s">
-        <v>916</v>
-      </c>
-      <c r="I351" s="47" t="s">
-        <v>915</v>
-      </c>
-      <c r="J351" s="45" t="s">
+      <c r="G351" s="35" t="s">
+        <v>914</v>
+      </c>
+      <c r="H351" s="35" t="s">
+        <v>913</v>
+      </c>
+      <c r="I351" s="35" t="s">
+        <v>912</v>
+      </c>
+      <c r="J351" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K351" s="25"/>
-      <c r="L351" s="45" t="s">
+      <c r="L351" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M351" s="45" t="s">
+      <c r="M351" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N351" s="45" t="s">
-        <v>914</v>
+      <c r="N351" s="33" t="s">
+        <v>911</v>
       </c>
       <c r="O351" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P351" s="45" t="s">
-        <v>857</v>
+      <c r="P351" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q351" s="25"/>
       <c r="R351" s="26"/>
@@ -19952,33 +19969,33 @@
       <c r="F352" s="23">
         <v>45062</v>
       </c>
-      <c r="G352" s="47" t="s">
-        <v>920</v>
-      </c>
-      <c r="H352" s="47" t="s">
-        <v>921</v>
-      </c>
-      <c r="I352" s="47" t="s">
-        <v>919</v>
-      </c>
-      <c r="J352" s="45" t="s">
+      <c r="G352" s="35" t="s">
+        <v>917</v>
+      </c>
+      <c r="H352" s="35" t="s">
+        <v>918</v>
+      </c>
+      <c r="I352" s="35" t="s">
+        <v>916</v>
+      </c>
+      <c r="J352" s="33" t="s">
         <v>488</v>
       </c>
       <c r="K352" s="25"/>
-      <c r="L352" s="45" t="s">
+      <c r="L352" s="33" t="s">
         <v>828</v>
       </c>
-      <c r="M352" s="45" t="s">
+      <c r="M352" s="33" t="s">
         <v>488</v>
       </c>
-      <c r="N352" s="45" t="s">
-        <v>918</v>
+      <c r="N352" s="33" t="s">
+        <v>915</v>
       </c>
       <c r="O352" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="P352" s="45" t="s">
-        <v>857</v>
+      <c r="P352" s="33" t="s">
+        <v>854</v>
       </c>
       <c r="Q352" s="25"/>
       <c r="R352" s="26"/>

</xml_diff>

<commit_message>
Modificato File come richiesto da fse-pnrr@innovazione.gov.it
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix-xis/v3_19_05/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix-xis/v3_19_05/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACCREDITAMENTO_FSE\GATEWAY\A1#111ELCO0000000\EL_CO_\Fenix-xis\v3_19_05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA858CD4-5EC3-4352-A350-E3EA607A42D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5EAD6B-6B3F-48CF-B0A5-4788E5D9D758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5385" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-192" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -4422,9 +4422,6 @@
     <t>SI, Da rivalidare</t>
   </si>
   <si>
-    <t>Rivalidazione in Backoffice</t>
-  </si>
-  <si>
     <t>Il sistema attende un numero di millisecondi configurabile (default 5000) Dopo tale tempo viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
   </si>
   <si>
@@ -4464,16 +4461,6 @@
     <t>2.16.840.1.113883.2.9.2.10.4.4.7102.6cf26d9d5440064a0ece43fe2aadb3bec28efe3a489f39f8b8adc64430b01b23.1ca402caf2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'languageCode'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected.Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
-    <t>[ERRORE-44| Il codice fiscale 'CCRRSA23E01I480j' c… deve essere costituito da 16 cifre [A-Z0-9]{16}]Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
-    <t>ERRORE-6| L'elemento ClinicalDocument/confidentialityCode DEVE avere l'attributo @code valorizzato con 'N' o 'V', e il @codeSystem='2.16.840.1.113883.5.25']
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
     <t>2023-05-16T16:28:15.842Z</t>
   </si>
   <si>
@@ -4486,10 +4473,6 @@
     <t>Occorre nuova Firma dopo correzzione</t>
   </si>
   <si>
-    <t>[ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ]
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
     <t>2186a9106df7f5b2</t>
   </si>
   <si>
@@ -4499,10 +4482,6 @@
     <t>2.16.840.1.113883.2.9.2.10.4.4.7102.15037f335c647502fef468ba84371e13e7a8302cbd0ba1bbaae05be80780ef9a.f865e6cced^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.10.4.4.7102.6001bef8bcba6ea80548af426a691339f94768ca41a6bd743b702cd6863e1277.00586856b8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -4512,10 +4491,6 @@
     <t>2023-05-16T16:42:26.439Z</t>
   </si>
   <si>
-    <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: L]
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
     <t>2023-05-16T16:46:00.061Z</t>
   </si>
   <si>
@@ -4525,10 +4500,6 @@
     <t>19e0acb9dc629c5a</t>
   </si>
   <si>
-    <t>[ERRORE-33a| L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR' ]
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.10.4.4.7102.d6af89b6583ec0ebdbcc8f4c6bda01247f49f90ba3edd3032a6f7c9ce3bce072.aae4c62df4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -4538,10 +4509,6 @@
     <t>2023-05-16T17:05:06.961Z</t>
   </si>
   <si>
-    <t>[ERRORE-38| inFulfillmentOf/order/priorityCode DEVE avere l'attributo '@codeSystem='2.16.840.1.113883.5.7' e @code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM' ]
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.10.4.4.7102.cdbc4636b86949d6cf77cabfa64f90c58827253e39c23c901f24a6108abc8264.e7170bb0e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -4551,10 +4518,6 @@
     <t>2023-05-16T17:11:45.063Z</t>
   </si>
   <si>
-    <t>ERROR: -1,-1 cvc-datatype-valid.1.2.3: '' is not a valid value of union type 'uid'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'root' on element 'id' is not valid with respect to its type, 'uid'.
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.10.4.4.7102.e0470ea447bed72b7c1a39651d635eb805c3b8a276110625aa7d7bcf62aa9b4d.4245d4370a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -4564,10 +4527,6 @@
     <t>2023-05-16T17:15:34.539Z</t>
   </si>
   <si>
-    <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.1 v2.73, Codes: null] 
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.10.4.4.7102.3de54a1313015f1376bc480182ce324bad056eb24804b972c9792504c3f5865c.82ff805730^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -4577,138 +4536,176 @@
     <t>2023-05-16T17:23:05.441Z</t>
   </si>
   <si>
-    <t>[ERRORE-b4| Sezione Referto: la sezione DEVE essere presente],[ERRORE-b5| Sezione Referto: la sezione DEVE contenere un elemento 'text'
+    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.1fe502b1550ffbfba0913bb1237a78bc64870543d2e478f1cad7420729b72092.13708c37f4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>76b0dbbf1d0d8cf2</t>
+  </si>
+  <si>
+    <t>2023-05-16T17:26:32.206Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.9c35861df8420979d6bccd1f7e3da045b6f61c5458bbf26fa49ea33e15055e1a.bc4d22cb79^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>9a1b100826652e6b</t>
+  </si>
+  <si>
+    <t>2023-05-16T17:31:32.872Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.31d274a867e36c65efe2dc312286c8dba3750faa67966f8dd10456ec7457fa1d.888ddc4a18^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>52d8937e5a497526</t>
+  </si>
+  <si>
+    <t>2023-05-16T17:36:05.894Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.bd6aa900419778b3887b6d9d0b92ec280812ef332575e02f781cc44f63eca3a7.959a834bd0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>7ab43f8d10d94460</t>
+  </si>
+  <si>
+    <t>2023-05-16T18:01:15.945Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.bd6aa900419778b3887b6d9d0b92ec280812ef332575e02f781cc44f63eca3a7.247203b8d5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>82232ed4798ae24e</t>
+  </si>
+  <si>
+    <t>2023-05-16T18:07:47.948Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.26b748869cedfe42582cb1508466766c00a9a72b3f570e2b43d9569523fd770f.cc2c28cc84^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>998e44fd8029053c</t>
+  </si>
+  <si>
+    <t>2023-05-16T18:13:16.075Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.26b748869cedfe42582cb1508466766c00a9a72b3f570e2b43d9569523fd770f.6c7bda8e39^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-16T18:16:46.245Z</t>
+  </si>
+  <si>
+    <t>c8b89067f95a1550</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.4a65b95f88aa526f9a0fc2bce3bebd5fc97cd1eae2ae3c55be7a09a52d59fb9d.41734ede70^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>3bc2b35a360cb74c</t>
+  </si>
+  <si>
+    <t>2023-05-16T18:25:16.520Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.79a6cbbe62ee646ca6fd59f47960547002e5eaf852329a0584755401db8e4219.102b3bbe03^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-16T18:28:32.108Z</t>
+  </si>
+  <si>
+    <t>3da1a208c48894f9</t>
+  </si>
+  <si>
+    <t>UNKNOWN_WORKFLOW_ID</t>
+  </si>
+  <si>
+    <t>9dcdbaaa9b0a140e</t>
+  </si>
+  <si>
+    <t>ee2620354d738c3f</t>
+  </si>
+  <si>
+    <t>2023-05-18T10:59:07.434Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il campo purpose_of_use non è valorizzato
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il campo action_id non è corretto
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Invalid content was found starting with element 'languageCode'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected.2</t>
+  </si>
+  <si>
+    <t>In automatico prima di inviare a fse o al repository viene tentata nuova validazione</t>
+  </si>
+  <si>
+    <t>Il codice fiscale 'CCRRSA23E01I480j' c… deve essere costituito da 16 cifre [A-Z0-9]{16}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'elemento ClinicalDocument/confidentialityCode DEVE avere l'attributo @code valorizzato con 'N' o 'V', e il @codeSystem='2.16.840.1.113883.5.25']
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: L]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR' ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> inFulfillmentOf/order/priorityCode DEVE avere l'attributo '@codeSystem='2.16.840.1.113883.5.7' e @code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM' ]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The value '' of attribute 'root' on element 'id' is not valid with respect to its type, 'uid'.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.1 v2.73, Codes: null] 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sezione Referto: la sezione DEVE essere presente],[ERRORE-b5| Sezione Referto: la sezione DEVE contenere un elemento 'text'
+</t>
+  </si>
+  <si>
+    <t>Sezione Quesito Diagnostico: la sezione DEVE contenere un elemento 'text']
 Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2]</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.1fe502b1550ffbfba0913bb1237a78bc64870543d2e478f1cad7420729b72092.13708c37f4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>76b0dbbf1d0d8cf2</t>
-  </si>
-  <si>
-    <t>2023-05-16T17:26:32.206Z</t>
-  </si>
-  <si>
-    <t>[ERRORE-b6| Sezione Quesito Diagnostico: la sezione DEVE contenere un elemento 'text']
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.9c35861df8420979d6bccd1f7e3da045b6f61c5458bbf26fa49ea33e15055e1a.bc4d22cb79^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>9a1b100826652e6b</t>
-  </si>
-  <si>
-    <t>2023-05-16T17:31:32.872Z</t>
-  </si>
-  <si>
-    <t>[ERRORE-b3| Sezione Prestazioni: la sezione DEVE contenere un elemento 'entry']
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.31d274a867e36c65efe2dc312286c8dba3750faa67966f8dd10456ec7457fa1d.888ddc4a18^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>52d8937e5a497526</t>
-  </si>
-  <si>
-    <t>2023-05-16T17:36:05.894Z</t>
-  </si>
-  <si>
-    <t>[ERRORE-b26| Sezione Storia Clinica: l'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato],[ERRORE-b27| Sezione Storia Clinica: l'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'high' valorizzato nel caso in cui il problema non sia più presente]
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.bd6aa900419778b3887b6d9d0b92ec280812ef332575e02f781cc44f63eca3a7.959a834bd0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>7ab43f8d10d94460</t>
-  </si>
-  <si>
-    <t>2023-05-16T18:01:15.945Z</t>
-  </si>
-  <si>
-    <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.111 v2.2.0, Codes: null]
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.bd6aa900419778b3887b6d9d0b92ec280812ef332575e02f781cc44f63eca3a7.247203b8d5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>82232ed4798ae24e</t>
-  </si>
-  <si>
-    <t>2023-05-16T18:07:47.948Z</t>
-  </si>
-  <si>
-    <t>ERRORE-b48| Sotto-sezione Allergie: l'elemento entry/act/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato],[ERRORE-b49| Sotto-sezione Allergie: l'elemento entry/act/effectiveTime/high deve essere presente nel caso in cui lo 'statusCode' sia 'completed'oppure'aborted']
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.26b748869cedfe42582cb1508466766c00a9a72b3f570e2b43d9569523fd770f.cc2c28cc84^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>998e44fd8029053c</t>
-  </si>
-  <si>
-    <t>2023-05-16T18:13:16.075Z</t>
-  </si>
-  <si>
-    <t>[ERRORE-b57| Sotto-sezione Allergie: entry/act/entryRelationship/observation deve contenere almeno un elemento 'participant']Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.26b748869cedfe42582cb1508466766c00a9a72b3f570e2b43d9569523fd770f.6c7bda8e39^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-16T18:16:46.245Z</t>
-  </si>
-  <si>
-    <t>c8b89067f95a1550</t>
-  </si>
-  <si>
-    <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: ABC123]Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.4a65b95f88aa526f9a0fc2bce3bebd5fc97cd1eae2ae3c55be7a09a52d59fb9d.41734ede70^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>3bc2b35a360cb74c</t>
-  </si>
-  <si>
-    <t>2023-05-16T18:25:16.520Z</t>
-  </si>
-  <si>
-    <t>[ERRORE-30| L'elemento ClinicalDocument/legalAuthenticator/signatureCode deve essere valorizzato con il codice "S" ]Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.7102.79a6cbbe62ee646ca6fd59f47960547002e5eaf852329a0584755401db8e4219.102b3bbe03^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-16T18:28:32.108Z</t>
-  </si>
-  <si>
-    <t>3da1a208c48894f9</t>
-  </si>
-  <si>
-    <t>UNKNOWN_WORKFLOW_ID</t>
-  </si>
-  <si>
-    <t>9dcdbaaa9b0a140e</t>
-  </si>
-  <si>
-    <t>Il campo purpose_of_use non è valorizzato
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
-    <t>ee2620354d738c3f</t>
-  </si>
-  <si>
-    <t>2023-05-18T10:59:07.434Z</t>
-  </si>
-  <si>
-    <t>Il campo action_id non è corretto
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
+    <t>[ERRORE-b3| Sezione Prestazioni: la sezione DEVE contenere un elemento 'entry'</t>
+  </si>
+  <si>
+    <t>[ERRORE-b26| Sezione Storia Clinica: l'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato],[ERRORE-b27| Sezione Storia Clinica: l'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'high' valorizzato nel caso in cui il problema non sia più presente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.111 v2.2.0, Codes: null]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sotto-sezione Allergie: l'elemento entry/act/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato],[ERRORE-b49| Sotto-sezione Allergie: l'elemento entry/act/effectiveTime/high deve essere presente nel caso in cui lo 'statusCode' sia 'completed'oppure'aborted'
+</t>
+  </si>
+  <si>
+    <t>Sotto-sezione Allergie: entry/act/entryRelationship/observation deve contenere almeno un elemento 'participant']</t>
+  </si>
+  <si>
+    <t>L'elemento ClinicalDocument/legalAuthenticator/signatureCode deve essere valorizzato con il codice "S"</t>
+  </si>
+  <si>
+    <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: ABC123]</t>
   </si>
 </sst>
 </file>
@@ -7613,10 +7610,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="M231" sqref="M231"/>
+      <selection pane="bottomRight" activeCell="O351" sqref="O351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -14861,10 +14858,10 @@
         <v>832</v>
       </c>
       <c r="H215" s="24" t="s">
-        <v>920</v>
+        <v>900</v>
       </c>
       <c r="I215" s="24" t="s">
-        <v>919</v>
+        <v>899</v>
       </c>
       <c r="J215" s="25" t="s">
         <v>488</v>
@@ -14877,13 +14874,13 @@
         <v>488</v>
       </c>
       <c r="N215" s="25" t="s">
-        <v>921</v>
+        <v>903</v>
       </c>
       <c r="O215" s="25" t="s">
         <v>833</v>
       </c>
       <c r="P215" s="25" t="s">
-        <v>834</v>
+        <v>906</v>
       </c>
       <c r="Q215" s="25"/>
       <c r="R215" s="26"/>
@@ -15150,13 +15147,13 @@
         <v>45064</v>
       </c>
       <c r="G223" s="24" t="s">
-        <v>923</v>
+        <v>902</v>
       </c>
       <c r="H223" s="24" t="s">
-        <v>922</v>
+        <v>901</v>
       </c>
       <c r="I223" s="24" t="s">
-        <v>919</v>
+        <v>899</v>
       </c>
       <c r="J223" s="25" t="s">
         <v>488</v>
@@ -15169,13 +15166,13 @@
         <v>488</v>
       </c>
       <c r="N223" s="33" t="s">
-        <v>924</v>
+        <v>904</v>
       </c>
       <c r="O223" s="25" t="s">
         <v>833</v>
       </c>
       <c r="P223" s="25" t="s">
-        <v>834</v>
+        <v>906</v>
       </c>
       <c r="Q223" s="25"/>
       <c r="R223" s="26"/>
@@ -15450,7 +15447,7 @@
         <v>45062</v>
       </c>
       <c r="G231" s="24" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="H231" s="24"/>
       <c r="I231" s="24"/>
@@ -15465,13 +15462,13 @@
         <v>488</v>
       </c>
       <c r="N231" s="33" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="O231" s="25" t="s">
         <v>833</v>
       </c>
       <c r="P231" s="25" t="s">
-        <v>834</v>
+        <v>906</v>
       </c>
       <c r="Q231" s="25"/>
       <c r="R231" s="26" t="s">
@@ -18840,13 +18837,13 @@
         <v>45062</v>
       </c>
       <c r="G330" s="24" t="s">
+        <v>836</v>
+      </c>
+      <c r="H330" s="24" t="s">
+        <v>838</v>
+      </c>
+      <c r="I330" s="24" t="s">
         <v>837</v>
-      </c>
-      <c r="H330" s="24" t="s">
-        <v>839</v>
-      </c>
-      <c r="I330" s="24" t="s">
-        <v>838</v>
       </c>
       <c r="J330" s="25" t="s">
         <v>488</v>
@@ -18888,7 +18885,7 @@
         <v>828</v>
       </c>
       <c r="K331" s="33" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="L331" s="25"/>
       <c r="M331" s="25"/>
@@ -18926,7 +18923,7 @@
         <v>828</v>
       </c>
       <c r="K332" s="25" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="L332" s="25"/>
       <c r="M332" s="25"/>
@@ -18964,7 +18961,7 @@
         <v>828</v>
       </c>
       <c r="K333" s="25" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="L333" s="25"/>
       <c r="M333" s="25"/>
@@ -18978,7 +18975,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="334" spans="1:20" ht="165.75" thickBot="1">
+    <row r="334" spans="1:20" ht="120.75" thickBot="1">
       <c r="A334" s="20">
         <v>151</v>
       </c>
@@ -18998,13 +18995,13 @@
         <v>45062</v>
       </c>
       <c r="G334" s="35" t="s">
+        <v>841</v>
+      </c>
+      <c r="H334" s="35" t="s">
         <v>842</v>
       </c>
-      <c r="H334" s="35" t="s">
+      <c r="I334" s="35" t="s">
         <v>843</v>
-      </c>
-      <c r="I334" s="35" t="s">
-        <v>844</v>
       </c>
       <c r="J334" s="25" t="s">
         <v>488</v>
@@ -19017,13 +19014,13 @@
         <v>488</v>
       </c>
       <c r="N334" s="33" t="s">
-        <v>848</v>
+        <v>905</v>
       </c>
       <c r="O334" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P334" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q334" s="25"/>
       <c r="R334" s="26"/>
@@ -19052,13 +19049,13 @@
         <v>45062</v>
       </c>
       <c r="G335" s="24" t="s">
+        <v>844</v>
+      </c>
+      <c r="H335" s="35" t="s">
         <v>845</v>
       </c>
-      <c r="H335" s="35" t="s">
+      <c r="I335" s="35" t="s">
         <v>846</v>
-      </c>
-      <c r="I335" s="35" t="s">
-        <v>847</v>
       </c>
       <c r="J335" s="33" t="s">
         <v>488</v>
@@ -19071,13 +19068,13 @@
         <v>488</v>
       </c>
       <c r="N335" s="25" t="s">
-        <v>849</v>
+        <v>907</v>
       </c>
       <c r="O335" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P335" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q335" s="25"/>
       <c r="R335" s="26"/>
@@ -19086,7 +19083,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="336" spans="1:20" ht="165.75" thickBot="1">
+    <row r="336" spans="1:20" ht="135.75" thickBot="1">
       <c r="A336" s="20">
         <v>153</v>
       </c>
@@ -19106,13 +19103,13 @@
         <v>45062</v>
       </c>
       <c r="G336" s="35" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="H336" s="35" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="I336" s="35" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="J336" s="33" t="s">
         <v>488</v>
@@ -19125,13 +19122,13 @@
         <v>488</v>
       </c>
       <c r="N336" s="33" t="s">
-        <v>850</v>
+        <v>908</v>
       </c>
       <c r="O336" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P336" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q336" s="25"/>
       <c r="R336" s="26"/>
@@ -19140,7 +19137,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="337" spans="1:20" ht="165.75" thickBot="1">
+    <row r="337" spans="1:20" ht="135.75" thickBot="1">
       <c r="A337" s="20">
         <v>154</v>
       </c>
@@ -19160,13 +19157,13 @@
         <v>45062</v>
       </c>
       <c r="G337" s="35" t="s">
-        <v>857</v>
+        <v>852</v>
       </c>
       <c r="H337" s="35" t="s">
-        <v>856</v>
+        <v>851</v>
       </c>
       <c r="I337" s="35" t="s">
-        <v>858</v>
+        <v>853</v>
       </c>
       <c r="J337" s="33" t="s">
         <v>488</v>
@@ -19179,13 +19176,13 @@
         <v>488</v>
       </c>
       <c r="N337" s="33" t="s">
-        <v>855</v>
+        <v>909</v>
       </c>
       <c r="O337" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P337" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q337" s="25"/>
       <c r="R337" s="26"/>
@@ -19214,13 +19211,13 @@
         <v>45062</v>
       </c>
       <c r="G338" s="35" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="H338" s="35" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="I338" s="35" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="J338" s="33" t="s">
         <v>488</v>
@@ -19233,13 +19230,13 @@
         <v>488</v>
       </c>
       <c r="N338" s="33" t="s">
-        <v>859</v>
+        <v>910</v>
       </c>
       <c r="O338" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P338" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q338" s="25"/>
       <c r="R338" s="26"/>
@@ -19268,13 +19265,13 @@
         <v>45062</v>
       </c>
       <c r="G339" s="35" t="s">
-        <v>864</v>
+        <v>857</v>
       </c>
       <c r="H339" s="24" t="s">
-        <v>866</v>
+        <v>859</v>
       </c>
       <c r="I339" s="35" t="s">
-        <v>865</v>
+        <v>858</v>
       </c>
       <c r="J339" s="33" t="s">
         <v>488</v>
@@ -19287,13 +19284,13 @@
         <v>488</v>
       </c>
       <c r="N339" s="33" t="s">
-        <v>863</v>
+        <v>911</v>
       </c>
       <c r="O339" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P339" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q339" s="25"/>
       <c r="R339" s="26"/>
@@ -19302,7 +19299,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="340" spans="1:20" ht="180.75" thickBot="1">
+    <row r="340" spans="1:20" ht="135.75" thickBot="1">
       <c r="A340" s="20">
         <v>157</v>
       </c>
@@ -19322,13 +19319,13 @@
         <v>45062</v>
       </c>
       <c r="G340" s="24" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="H340" s="24" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="I340" s="24" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="J340" s="33" t="s">
         <v>488</v>
@@ -19341,13 +19338,13 @@
         <v>488</v>
       </c>
       <c r="N340" s="25" t="s">
-        <v>867</v>
+        <v>912</v>
       </c>
       <c r="O340" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P340" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q340" s="25"/>
       <c r="R340" s="26"/>
@@ -19356,7 +19353,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="341" spans="1:20" ht="180.75" thickBot="1">
+    <row r="341" spans="1:20" ht="135.75" thickBot="1">
       <c r="A341" s="20">
         <v>158</v>
       </c>
@@ -19376,13 +19373,13 @@
         <v>45062</v>
       </c>
       <c r="G341" s="35" t="s">
-        <v>874</v>
+        <v>865</v>
       </c>
       <c r="H341" s="35" t="s">
-        <v>873</v>
+        <v>864</v>
       </c>
       <c r="I341" s="35" t="s">
-        <v>872</v>
+        <v>863</v>
       </c>
       <c r="J341" s="33" t="s">
         <v>488</v>
@@ -19395,13 +19392,13 @@
         <v>488</v>
       </c>
       <c r="N341" s="33" t="s">
-        <v>871</v>
+        <v>913</v>
       </c>
       <c r="O341" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P341" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q341" s="25"/>
       <c r="R341" s="26"/>
@@ -19410,7 +19407,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="342" spans="1:20" ht="180.75" thickBot="1">
+    <row r="342" spans="1:20" ht="120.75" thickBot="1">
       <c r="A342" s="20">
         <v>159</v>
       </c>
@@ -19430,13 +19427,13 @@
         <v>45062</v>
       </c>
       <c r="G342" s="35" t="s">
-        <v>878</v>
+        <v>868</v>
       </c>
       <c r="H342" s="35" t="s">
-        <v>877</v>
+        <v>867</v>
       </c>
       <c r="I342" s="35" t="s">
-        <v>876</v>
+        <v>866</v>
       </c>
       <c r="J342" s="33" t="s">
         <v>488</v>
@@ -19449,13 +19446,13 @@
         <v>488</v>
       </c>
       <c r="N342" s="33" t="s">
-        <v>875</v>
+        <v>914</v>
       </c>
       <c r="O342" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P342" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q342" s="25"/>
       <c r="R342" s="26"/>
@@ -19464,7 +19461,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="343" spans="1:20" ht="150.75" thickBot="1">
+    <row r="343" spans="1:20" ht="120.75" thickBot="1">
       <c r="A343" s="20">
         <v>160</v>
       </c>
@@ -19484,13 +19481,13 @@
         <v>45062</v>
       </c>
       <c r="G343" s="35" t="s">
-        <v>882</v>
+        <v>871</v>
       </c>
       <c r="H343" s="35" t="s">
-        <v>881</v>
+        <v>870</v>
       </c>
       <c r="I343" s="35" t="s">
-        <v>880</v>
+        <v>869</v>
       </c>
       <c r="J343" s="33" t="s">
         <v>488</v>
@@ -19503,13 +19500,13 @@
         <v>488</v>
       </c>
       <c r="N343" s="33" t="s">
-        <v>879</v>
+        <v>915</v>
       </c>
       <c r="O343" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P343" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q343" s="25"/>
       <c r="R343" s="26"/>
@@ -19518,7 +19515,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="344" spans="1:20" ht="165.75" thickBot="1">
+    <row r="344" spans="1:20" ht="135.75" thickBot="1">
       <c r="A344" s="20">
         <v>161</v>
       </c>
@@ -19538,13 +19535,13 @@
         <v>45062</v>
       </c>
       <c r="G344" s="35" t="s">
-        <v>886</v>
+        <v>874</v>
       </c>
       <c r="H344" s="35" t="s">
-        <v>885</v>
+        <v>873</v>
       </c>
       <c r="I344" s="35" t="s">
-        <v>884</v>
+        <v>872</v>
       </c>
       <c r="J344" s="33" t="s">
         <v>488</v>
@@ -19557,13 +19554,13 @@
         <v>488</v>
       </c>
       <c r="N344" s="33" t="s">
-        <v>883</v>
+        <v>916</v>
       </c>
       <c r="O344" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P344" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q344" s="25"/>
       <c r="R344" s="26"/>
@@ -19592,13 +19589,13 @@
         <v>45062</v>
       </c>
       <c r="G345" s="35" t="s">
-        <v>890</v>
+        <v>877</v>
       </c>
       <c r="H345" s="35" t="s">
-        <v>889</v>
+        <v>876</v>
       </c>
       <c r="I345" s="35" t="s">
-        <v>888</v>
+        <v>875</v>
       </c>
       <c r="J345" s="33" t="s">
         <v>488</v>
@@ -19611,13 +19608,13 @@
         <v>488</v>
       </c>
       <c r="N345" s="33" t="s">
-        <v>887</v>
+        <v>917</v>
       </c>
       <c r="O345" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P345" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q345" s="25"/>
       <c r="R345" s="26"/>
@@ -19646,13 +19643,13 @@
         <v>45062</v>
       </c>
       <c r="G346" s="35" t="s">
-        <v>894</v>
+        <v>880</v>
       </c>
       <c r="H346" s="35" t="s">
-        <v>893</v>
+        <v>879</v>
       </c>
       <c r="I346" s="35" t="s">
-        <v>892</v>
+        <v>878</v>
       </c>
       <c r="J346" s="33" t="s">
         <v>488</v>
@@ -19665,13 +19662,13 @@
         <v>488</v>
       </c>
       <c r="N346" s="33" t="s">
-        <v>891</v>
+        <v>918</v>
       </c>
       <c r="O346" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P346" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q346" s="25"/>
       <c r="R346" s="26"/>
@@ -19680,7 +19677,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="347" spans="1:20" ht="240.75" thickBot="1">
+    <row r="347" spans="1:20" ht="150.75" thickBot="1">
       <c r="A347" s="20">
         <v>164</v>
       </c>
@@ -19700,13 +19697,13 @@
         <v>45062</v>
       </c>
       <c r="G347" s="35" t="s">
-        <v>898</v>
+        <v>883</v>
       </c>
       <c r="H347" s="35" t="s">
-        <v>897</v>
+        <v>882</v>
       </c>
       <c r="I347" s="35" t="s">
-        <v>896</v>
+        <v>881</v>
       </c>
       <c r="J347" s="33" t="s">
         <v>488</v>
@@ -19719,13 +19716,13 @@
         <v>488</v>
       </c>
       <c r="N347" s="33" t="s">
-        <v>895</v>
+        <v>919</v>
       </c>
       <c r="O347" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P347" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q347" s="25"/>
       <c r="R347" s="26"/>
@@ -19734,7 +19731,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="348" spans="1:20" ht="150">
+    <row r="348" spans="1:20" ht="135">
       <c r="A348" s="20">
         <v>165</v>
       </c>
@@ -19754,13 +19751,13 @@
         <v>45062</v>
       </c>
       <c r="G348" s="35" t="s">
-        <v>902</v>
+        <v>886</v>
       </c>
       <c r="H348" s="35" t="s">
-        <v>901</v>
+        <v>885</v>
       </c>
       <c r="I348" s="35" t="s">
-        <v>900</v>
+        <v>884</v>
       </c>
       <c r="J348" s="33" t="s">
         <v>488</v>
@@ -19773,13 +19770,13 @@
         <v>488</v>
       </c>
       <c r="N348" s="33" t="s">
-        <v>899</v>
+        <v>920</v>
       </c>
       <c r="O348" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P348" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q348" s="25"/>
       <c r="R348" s="26"/>
@@ -19788,7 +19785,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="349" spans="1:20" ht="240">
+    <row r="349" spans="1:20" ht="150">
       <c r="A349" s="20">
         <v>166</v>
       </c>
@@ -19808,13 +19805,13 @@
         <v>45062</v>
       </c>
       <c r="G349" s="35" t="s">
-        <v>906</v>
+        <v>889</v>
       </c>
       <c r="H349" s="35" t="s">
-        <v>905</v>
+        <v>888</v>
       </c>
       <c r="I349" s="35" t="s">
-        <v>904</v>
+        <v>887</v>
       </c>
       <c r="J349" s="33" t="s">
         <v>488</v>
@@ -19827,13 +19824,13 @@
         <v>488</v>
       </c>
       <c r="N349" s="33" t="s">
-        <v>903</v>
+        <v>921</v>
       </c>
       <c r="O349" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P349" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q349" s="25"/>
       <c r="R349" s="26"/>
@@ -19862,13 +19859,13 @@
         <v>45062</v>
       </c>
       <c r="G350" s="24" t="s">
-        <v>909</v>
+        <v>891</v>
       </c>
       <c r="H350" s="24" t="s">
-        <v>910</v>
+        <v>892</v>
       </c>
       <c r="I350" s="24" t="s">
-        <v>908</v>
+        <v>890</v>
       </c>
       <c r="J350" s="33" t="s">
         <v>488</v>
@@ -19881,13 +19878,13 @@
         <v>488</v>
       </c>
       <c r="N350" s="33" t="s">
-        <v>907</v>
+        <v>922</v>
       </c>
       <c r="O350" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P350" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q350" s="25"/>
       <c r="R350" s="26"/>
@@ -19916,13 +19913,13 @@
         <v>45062</v>
       </c>
       <c r="G351" s="35" t="s">
-        <v>914</v>
+        <v>895</v>
       </c>
       <c r="H351" s="35" t="s">
-        <v>913</v>
+        <v>894</v>
       </c>
       <c r="I351" s="35" t="s">
-        <v>912</v>
+        <v>893</v>
       </c>
       <c r="J351" s="33" t="s">
         <v>488</v>
@@ -19935,13 +19932,13 @@
         <v>488</v>
       </c>
       <c r="N351" s="33" t="s">
-        <v>911</v>
+        <v>924</v>
       </c>
       <c r="O351" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P351" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q351" s="25"/>
       <c r="R351" s="26"/>
@@ -19970,13 +19967,13 @@
         <v>45062</v>
       </c>
       <c r="G352" s="35" t="s">
-        <v>917</v>
+        <v>897</v>
       </c>
       <c r="H352" s="35" t="s">
-        <v>918</v>
+        <v>898</v>
       </c>
       <c r="I352" s="35" t="s">
-        <v>916</v>
+        <v>896</v>
       </c>
       <c r="J352" s="33" t="s">
         <v>488</v>
@@ -19989,13 +19986,13 @@
         <v>488</v>
       </c>
       <c r="N352" s="33" t="s">
-        <v>915</v>
+        <v>923</v>
       </c>
       <c r="O352" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P352" s="33" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="Q352" s="25"/>
       <c r="R352" s="26"/>

</xml_diff>

<commit_message>
risottomettessa la check-list, dettagliando nella stessa colonna per i casi con:
•	ID 32, 40, l’intervento effettuato dal backoffice prima di inviare il documento al FSE o al repository
•	ID 151, 152, 153, 154, 155, 156, 157, 158, 159 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, la procedura adottata per la risoluzione dell’errore e le modalità di invio successivo del documento al FSE, considerato che si sta descrivendo la gestione dell’errore nel processo di validazione.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix-xis/v3_19_05/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix-xis/v3_19_05/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACCREDITAMENTO_FSE\GATEWAY\A1#111ELCO0000000\EL_CO_\Fenix-xis\v3_19_05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5EAD6B-6B3F-48CF-B0A5-4788E5D9D758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8356EB-9A92-404F-AAFD-1D288FDCBD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-192" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,19 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$374</definedName>
     <definedName name="filtro" localSheetId="2">TestCases!$A$9:$S$203</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mhUlYP9yzNmk4f07XMJovPPUaqOhw=="/>
     </ext>
@@ -4419,9 +4430,6 @@
     <t>2023-05-16T13:04:54.185Z</t>
   </si>
   <si>
-    <t>SI, Da rivalidare</t>
-  </si>
-  <si>
     <t>Il sistema attende un numero di millisecondi configurabile (default 5000) Dopo tale tempo viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
   </si>
   <si>
@@ -4468,9 +4476,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.10.4.4.7102.3765a272cfc46b9f8aeb93866e925484fc7049222920a714d07437f1e53a99e9.8efb85e9e4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Occorre nuova Firma dopo correzzione</t>
   </si>
   <si>
     <t>2186a9106df7f5b2</t>
@@ -4706,6 +4711,12 @@
   </si>
   <si>
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: ABC123]</t>
+  </si>
+  <si>
+    <t>Tramite apposito cruscotto sul software di BI potrà essere preso in carico l'errore, corretto il campo da interfaccia e reinviato il referto</t>
+  </si>
+  <si>
+    <t>Tramite apposito cruscotto sul software di BI potrà essere preso in carico l'errore, corretto il campo da interfaccia e reinviato il referto  Occorre nuova Firma dopo correzzione in quanto il dato è contenuto all'interno del CDA2</t>
   </si>
 </sst>
 </file>
@@ -7610,10 +7621,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="O351" sqref="O351"/>
+      <selection pane="bottomRight" activeCell="P352" sqref="P352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -14858,10 +14869,10 @@
         <v>832</v>
       </c>
       <c r="H215" s="24" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="I215" s="24" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="J215" s="25" t="s">
         <v>488</v>
@@ -14874,13 +14885,13 @@
         <v>488</v>
       </c>
       <c r="N215" s="25" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="O215" s="25" t="s">
-        <v>833</v>
+        <v>488</v>
       </c>
       <c r="P215" s="25" t="s">
-        <v>906</v>
+        <v>923</v>
       </c>
       <c r="Q215" s="25"/>
       <c r="R215" s="26"/>
@@ -15147,13 +15158,13 @@
         <v>45064</v>
       </c>
       <c r="G223" s="24" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="H223" s="24" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="I223" s="24" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="J223" s="25" t="s">
         <v>488</v>
@@ -15166,13 +15177,13 @@
         <v>488</v>
       </c>
       <c r="N223" s="33" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="O223" s="25" t="s">
-        <v>833</v>
+        <v>488</v>
       </c>
       <c r="P223" s="25" t="s">
-        <v>906</v>
+        <v>923</v>
       </c>
       <c r="Q223" s="25"/>
       <c r="R223" s="26"/>
@@ -15447,7 +15458,7 @@
         <v>45062</v>
       </c>
       <c r="G231" s="24" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="H231" s="24"/>
       <c r="I231" s="24"/>
@@ -15462,13 +15473,13 @@
         <v>488</v>
       </c>
       <c r="N231" s="33" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="O231" s="25" t="s">
-        <v>833</v>
+        <v>488</v>
       </c>
       <c r="P231" s="25" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="Q231" s="25"/>
       <c r="R231" s="26" t="s">
@@ -18837,13 +18848,13 @@
         <v>45062</v>
       </c>
       <c r="G330" s="24" t="s">
+        <v>835</v>
+      </c>
+      <c r="H330" s="24" t="s">
+        <v>837</v>
+      </c>
+      <c r="I330" s="24" t="s">
         <v>836</v>
-      </c>
-      <c r="H330" s="24" t="s">
-        <v>838</v>
-      </c>
-      <c r="I330" s="24" t="s">
-        <v>837</v>
       </c>
       <c r="J330" s="25" t="s">
         <v>488</v>
@@ -18885,7 +18896,7 @@
         <v>828</v>
       </c>
       <c r="K331" s="33" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="L331" s="25"/>
       <c r="M331" s="25"/>
@@ -18923,7 +18934,7 @@
         <v>828</v>
       </c>
       <c r="K332" s="25" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="L332" s="25"/>
       <c r="M332" s="25"/>
@@ -18961,7 +18972,7 @@
         <v>828</v>
       </c>
       <c r="K333" s="25" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="L333" s="25"/>
       <c r="M333" s="25"/>
@@ -18975,7 +18986,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="334" spans="1:20" ht="120.75" thickBot="1">
+    <row r="334" spans="1:20" ht="135.75" thickBot="1">
       <c r="A334" s="20">
         <v>151</v>
       </c>
@@ -18995,13 +19006,13 @@
         <v>45062</v>
       </c>
       <c r="G334" s="35" t="s">
+        <v>840</v>
+      </c>
+      <c r="H334" s="35" t="s">
         <v>841</v>
       </c>
-      <c r="H334" s="35" t="s">
+      <c r="I334" s="35" t="s">
         <v>842</v>
-      </c>
-      <c r="I334" s="35" t="s">
-        <v>843</v>
       </c>
       <c r="J334" s="25" t="s">
         <v>488</v>
@@ -19014,13 +19025,13 @@
         <v>488</v>
       </c>
       <c r="N334" s="33" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="O334" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P334" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q334" s="25"/>
       <c r="R334" s="26"/>
@@ -19049,13 +19060,13 @@
         <v>45062</v>
       </c>
       <c r="G335" s="24" t="s">
+        <v>843</v>
+      </c>
+      <c r="H335" s="35" t="s">
         <v>844</v>
       </c>
-      <c r="H335" s="35" t="s">
+      <c r="I335" s="35" t="s">
         <v>845</v>
-      </c>
-      <c r="I335" s="35" t="s">
-        <v>846</v>
       </c>
       <c r="J335" s="33" t="s">
         <v>488</v>
@@ -19068,13 +19079,13 @@
         <v>488</v>
       </c>
       <c r="N335" s="25" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="O335" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P335" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q335" s="25"/>
       <c r="R335" s="26"/>
@@ -19103,13 +19114,13 @@
         <v>45062</v>
       </c>
       <c r="G336" s="35" t="s">
+        <v>846</v>
+      </c>
+      <c r="H336" s="35" t="s">
         <v>847</v>
       </c>
-      <c r="H336" s="35" t="s">
+      <c r="I336" s="35" t="s">
         <v>848</v>
-      </c>
-      <c r="I336" s="35" t="s">
-        <v>849</v>
       </c>
       <c r="J336" s="33" t="s">
         <v>488</v>
@@ -19122,13 +19133,13 @@
         <v>488</v>
       </c>
       <c r="N336" s="33" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="O336" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P336" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q336" s="25"/>
       <c r="R336" s="26"/>
@@ -19157,13 +19168,13 @@
         <v>45062</v>
       </c>
       <c r="G337" s="35" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="H337" s="35" t="s">
+        <v>849</v>
+      </c>
+      <c r="I337" s="35" t="s">
         <v>851</v>
-      </c>
-      <c r="I337" s="35" t="s">
-        <v>853</v>
       </c>
       <c r="J337" s="33" t="s">
         <v>488</v>
@@ -19176,13 +19187,13 @@
         <v>488</v>
       </c>
       <c r="N337" s="33" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="O337" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P337" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q337" s="25"/>
       <c r="R337" s="26"/>
@@ -19211,13 +19222,13 @@
         <v>45062</v>
       </c>
       <c r="G338" s="35" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="H338" s="35" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="I338" s="35" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="J338" s="33" t="s">
         <v>488</v>
@@ -19230,13 +19241,13 @@
         <v>488</v>
       </c>
       <c r="N338" s="33" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="O338" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P338" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q338" s="25"/>
       <c r="R338" s="26"/>
@@ -19265,13 +19276,13 @@
         <v>45062</v>
       </c>
       <c r="G339" s="35" t="s">
+        <v>855</v>
+      </c>
+      <c r="H339" s="24" t="s">
         <v>857</v>
       </c>
-      <c r="H339" s="24" t="s">
-        <v>859</v>
-      </c>
       <c r="I339" s="35" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="J339" s="33" t="s">
         <v>488</v>
@@ -19284,13 +19295,13 @@
         <v>488</v>
       </c>
       <c r="N339" s="33" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="O339" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P339" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q339" s="25"/>
       <c r="R339" s="26"/>
@@ -19319,13 +19330,13 @@
         <v>45062</v>
       </c>
       <c r="G340" s="24" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="H340" s="24" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="I340" s="24" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="J340" s="33" t="s">
         <v>488</v>
@@ -19338,13 +19349,13 @@
         <v>488</v>
       </c>
       <c r="N340" s="25" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="O340" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P340" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q340" s="25"/>
       <c r="R340" s="26"/>
@@ -19373,13 +19384,13 @@
         <v>45062</v>
       </c>
       <c r="G341" s="35" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="H341" s="35" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="I341" s="35" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="J341" s="33" t="s">
         <v>488</v>
@@ -19392,13 +19403,13 @@
         <v>488</v>
       </c>
       <c r="N341" s="33" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="O341" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P341" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q341" s="25"/>
       <c r="R341" s="26"/>
@@ -19407,7 +19418,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="342" spans="1:20" ht="120.75" thickBot="1">
+    <row r="342" spans="1:20" ht="135.75" thickBot="1">
       <c r="A342" s="20">
         <v>159</v>
       </c>
@@ -19427,13 +19438,13 @@
         <v>45062</v>
       </c>
       <c r="G342" s="35" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="H342" s="35" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="I342" s="35" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="J342" s="33" t="s">
         <v>488</v>
@@ -19446,13 +19457,13 @@
         <v>488</v>
       </c>
       <c r="N342" s="33" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="O342" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P342" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q342" s="25"/>
       <c r="R342" s="26"/>
@@ -19461,7 +19472,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="343" spans="1:20" ht="120.75" thickBot="1">
+    <row r="343" spans="1:20" ht="135.75" thickBot="1">
       <c r="A343" s="20">
         <v>160</v>
       </c>
@@ -19481,13 +19492,13 @@
         <v>45062</v>
       </c>
       <c r="G343" s="35" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="H343" s="35" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="I343" s="35" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="J343" s="33" t="s">
         <v>488</v>
@@ -19500,13 +19511,13 @@
         <v>488</v>
       </c>
       <c r="N343" s="33" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="O343" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P343" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q343" s="25"/>
       <c r="R343" s="26"/>
@@ -19535,13 +19546,13 @@
         <v>45062</v>
       </c>
       <c r="G344" s="35" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="H344" s="35" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="I344" s="35" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="J344" s="33" t="s">
         <v>488</v>
@@ -19554,13 +19565,13 @@
         <v>488</v>
       </c>
       <c r="N344" s="33" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="O344" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P344" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q344" s="25"/>
       <c r="R344" s="26"/>
@@ -19589,13 +19600,13 @@
         <v>45062</v>
       </c>
       <c r="G345" s="35" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="H345" s="35" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="I345" s="35" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="J345" s="33" t="s">
         <v>488</v>
@@ -19608,13 +19619,13 @@
         <v>488</v>
       </c>
       <c r="N345" s="33" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="O345" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P345" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q345" s="25"/>
       <c r="R345" s="26"/>
@@ -19643,13 +19654,13 @@
         <v>45062</v>
       </c>
       <c r="G346" s="35" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="H346" s="35" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="I346" s="35" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="J346" s="33" t="s">
         <v>488</v>
@@ -19662,13 +19673,13 @@
         <v>488</v>
       </c>
       <c r="N346" s="33" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="O346" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P346" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q346" s="25"/>
       <c r="R346" s="26"/>
@@ -19697,13 +19708,13 @@
         <v>45062</v>
       </c>
       <c r="G347" s="35" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H347" s="35" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="I347" s="35" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="J347" s="33" t="s">
         <v>488</v>
@@ -19716,13 +19727,13 @@
         <v>488</v>
       </c>
       <c r="N347" s="33" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="O347" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P347" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q347" s="25"/>
       <c r="R347" s="26"/>
@@ -19751,13 +19762,13 @@
         <v>45062</v>
       </c>
       <c r="G348" s="35" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="H348" s="35" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="I348" s="35" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="J348" s="33" t="s">
         <v>488</v>
@@ -19770,13 +19781,13 @@
         <v>488</v>
       </c>
       <c r="N348" s="33" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="O348" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P348" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q348" s="25"/>
       <c r="R348" s="26"/>
@@ -19805,13 +19816,13 @@
         <v>45062</v>
       </c>
       <c r="G349" s="35" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="H349" s="35" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="I349" s="35" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="J349" s="33" t="s">
         <v>488</v>
@@ -19824,13 +19835,13 @@
         <v>488</v>
       </c>
       <c r="N349" s="33" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="O349" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P349" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q349" s="25"/>
       <c r="R349" s="26"/>
@@ -19859,13 +19870,13 @@
         <v>45062</v>
       </c>
       <c r="G350" s="24" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="H350" s="24" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="I350" s="24" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="J350" s="33" t="s">
         <v>488</v>
@@ -19878,13 +19889,13 @@
         <v>488</v>
       </c>
       <c r="N350" s="33" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="O350" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P350" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q350" s="25"/>
       <c r="R350" s="26"/>
@@ -19913,13 +19924,13 @@
         <v>45062</v>
       </c>
       <c r="G351" s="35" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="H351" s="35" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="I351" s="35" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="J351" s="33" t="s">
         <v>488</v>
@@ -19932,13 +19943,13 @@
         <v>488</v>
       </c>
       <c r="N351" s="33" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="O351" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P351" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q351" s="25"/>
       <c r="R351" s="26"/>
@@ -19967,13 +19978,13 @@
         <v>45062</v>
       </c>
       <c r="G352" s="35" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="H352" s="35" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="I352" s="35" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="J352" s="33" t="s">
         <v>488</v>
@@ -19986,13 +19997,13 @@
         <v>488</v>
       </c>
       <c r="N352" s="33" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="O352" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P352" s="33" t="s">
-        <v>850</v>
+        <v>924</v>
       </c>
       <c r="Q352" s="25"/>
       <c r="R352" s="26"/>

</xml_diff>